<commit_message>
Listo tif y rastro
</commit_message>
<xml_diff>
--- a/Documentos/Datos.xlsx
+++ b/Documentos/Datos.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7896"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7896" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rastros(TIF)" sheetId="1" r:id="rId1"/>
-    <sheet name="Rastros (Rastro)" sheetId="5" r:id="rId2"/>
+    <sheet name="Rastros(Rastro)" sheetId="5" r:id="rId2"/>
     <sheet name="Grupo de mercancía" sheetId="2" r:id="rId3"/>
     <sheet name="Sitio de inspección" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -5608,18 +5608,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5627,6 +5615,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5936,7 +5936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -5970,128 +5970,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="1" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="33" t="s">
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="29" t="s">
         <v>1117</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="31" t="s">
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="27" t="s">
         <v>967</v>
       </c>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
     </row>
     <row r="2" spans="1:40" s="1" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="27" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27" t="s">
+      <c r="W2" s="30"/>
+      <c r="X2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27" t="s">
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27" t="s">
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27" t="s">
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="27" t="s">
+      <c r="AE2" s="30"/>
+      <c r="AF2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="27" t="s">
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
     </row>
     <row r="3" spans="1:40" s="1" customFormat="1" ht="24" customHeight="1">
       <c r="A3" s="25" t="s">
@@ -6100,10 +6100,10 @@
       <c r="B3" s="25" t="s">
         <v>1769</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
@@ -6125,8 +6125,8 @@
       <c r="M3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="27"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="30"/>
       <c r="P3" s="18" t="s">
         <v>19</v>
       </c>
@@ -6142,7 +6142,7 @@
       <c r="T3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="33"/>
+      <c r="U3" s="29"/>
       <c r="V3" s="3" t="s">
         <v>24</v>
       </c>
@@ -16830,6 +16830,16 @@
     <filterColumn colId="38" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:M2"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:T2"/>
     <mergeCell ref="AJ1:AN2"/>
     <mergeCell ref="U1:U3"/>
     <mergeCell ref="V1:AI1"/>
@@ -16840,16 +16850,6 @@
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:M2"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="P1:T2"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O22" r:id="rId1"/>
@@ -16963,8 +16963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN103"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL4" sqref="AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -16990,134 +16990,134 @@
     <col min="21" max="21" width="15.5546875" style="5" customWidth="1"/>
     <col min="22" max="35" width="12.77734375" style="5" customWidth="1"/>
     <col min="36" max="37" width="8.88671875" style="5"/>
-    <col min="38" max="38" width="13.77734375" style="5" customWidth="1"/>
+    <col min="38" max="38" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="39" max="40" width="17.6640625" style="5" customWidth="1"/>
     <col min="41" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="1" customFormat="1" ht="23.4" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="33" t="s">
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="29" t="s">
         <v>1117</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="31" t="s">
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="27" t="s">
         <v>967</v>
       </c>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
     </row>
     <row r="2" spans="1:40" s="1" customFormat="1" ht="23.4" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="27" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27" t="s">
+      <c r="W2" s="30"/>
+      <c r="X2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27" t="s">
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27" t="s">
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27" t="s">
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="27" t="s">
+      <c r="AE2" s="30"/>
+      <c r="AF2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="27" t="s">
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
     </row>
     <row r="3" spans="1:40" s="1" customFormat="1" ht="23.4" customHeight="1">
       <c r="A3" s="25" t="s">
@@ -17126,10 +17126,10 @@
       <c r="B3" s="25" t="s">
         <v>1769</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="20" t="s">
         <v>12</v>
       </c>
@@ -17151,8 +17151,8 @@
       <c r="M3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="27"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="30"/>
       <c r="P3" s="21" t="s">
         <v>19</v>
       </c>
@@ -17168,7 +17168,7 @@
       <c r="T3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="33"/>
+      <c r="U3" s="29"/>
       <c r="V3" s="19" t="s">
         <v>24</v>
       </c>
@@ -27827,17 +27827,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="G1:M2"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="P1:T2"/>
-    <mergeCell ref="U1:U3"/>
     <mergeCell ref="AJ1:AN2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -27847,6 +27836,17 @@
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="V1:AI1"/>
+    <mergeCell ref="G1:M2"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:T2"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O22" r:id="rId1"/>
@@ -27978,10 +27978,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="35.4" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
@@ -28001,8 +28001,8 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="4" t="s">
         <v>564</v>
       </c>
@@ -30347,65 +30347,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="27" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Y1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="Z1" s="30" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="10" t="s">
         <v>48</v>
       </c>
@@ -30448,13 +30448,13 @@
       <c r="S2" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="25" t="s">
@@ -36854,11 +36854,6 @@
   </sheetData>
   <autoFilter ref="A2:Z102"/>
   <mergeCells count="13">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
@@ -36867,6 +36862,11 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:S1"/>
     <mergeCell ref="T1:T2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Grupo de Mercancias listo 100%
</commit_message>
<xml_diff>
--- a/Documentos/Datos.xlsx
+++ b/Documentos/Datos.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7896" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7896" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rastros(TIF)" sheetId="1" r:id="rId1"/>
     <sheet name="Rastros(Rastro)" sheetId="5" r:id="rId2"/>
-    <sheet name="Grupo de mercancía" sheetId="2" r:id="rId3"/>
+    <sheet name="Grupo_mercancia" sheetId="2" r:id="rId3"/>
     <sheet name="Sitio de inspección" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Grupo de mercancía'!$A$1:$G$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Grupo_mercancia!$A$1:$G$101</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Rastros(TIF)'!$A$1:$AN$103</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sitio de inspección'!$A$2:$Z$102</definedName>
   </definedNames>
@@ -5608,6 +5608,18 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5615,18 +5627,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5970,128 +5970,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="1" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31" t="s">
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="29" t="s">
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="33" t="s">
         <v>1117</v>
       </c>
-      <c r="V1" s="30" t="s">
+      <c r="V1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="27" t="s">
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="31" t="s">
         <v>967</v>
       </c>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
     </row>
     <row r="2" spans="1:40" s="1" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="30" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30" t="s">
+      <c r="W2" s="27"/>
+      <c r="X2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30" t="s">
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30" t="s">
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30" t="s">
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30" t="s">
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30" t="s">
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
+      <c r="AI2" s="27"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
     </row>
     <row r="3" spans="1:40" s="1" customFormat="1" ht="24" customHeight="1">
       <c r="A3" s="25" t="s">
@@ -6100,10 +6100,10 @@
       <c r="B3" s="25" t="s">
         <v>1769</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
@@ -6125,8 +6125,8 @@
       <c r="M3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="31"/>
-      <c r="O3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="27"/>
       <c r="P3" s="18" t="s">
         <v>19</v>
       </c>
@@ -6142,7 +6142,7 @@
       <c r="T3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="29"/>
+      <c r="U3" s="33"/>
       <c r="V3" s="3" t="s">
         <v>24</v>
       </c>
@@ -16830,16 +16830,6 @@
     <filterColumn colId="38" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:M2"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="P1:T2"/>
     <mergeCell ref="AJ1:AN2"/>
     <mergeCell ref="U1:U3"/>
     <mergeCell ref="V1:AI1"/>
@@ -16850,6 +16840,16 @@
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:M2"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:T2"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O22" r:id="rId1"/>
@@ -16963,7 +16963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AL4" sqref="AL4"/>
     </sheetView>
   </sheetViews>
@@ -16996,128 +16996,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="1" customFormat="1" ht="23.4" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31" t="s">
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="29" t="s">
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="33" t="s">
         <v>1117</v>
       </c>
-      <c r="V1" s="30" t="s">
+      <c r="V1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="27" t="s">
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="31" t="s">
         <v>967</v>
       </c>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
     </row>
     <row r="2" spans="1:40" s="1" customFormat="1" ht="23.4" customHeight="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="30" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30" t="s">
+      <c r="W2" s="27"/>
+      <c r="X2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30" t="s">
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30" t="s">
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30" t="s">
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30" t="s">
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30" t="s">
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
+      <c r="AI2" s="27"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
     </row>
     <row r="3" spans="1:40" s="1" customFormat="1" ht="23.4" customHeight="1">
       <c r="A3" s="25" t="s">
@@ -17126,10 +17126,10 @@
       <c r="B3" s="25" t="s">
         <v>1769</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="20" t="s">
         <v>12</v>
       </c>
@@ -17151,8 +17151,8 @@
       <c r="M3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="31"/>
-      <c r="O3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="27"/>
       <c r="P3" s="21" t="s">
         <v>19</v>
       </c>
@@ -17168,7 +17168,7 @@
       <c r="T3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="29"/>
+      <c r="U3" s="33"/>
       <c r="V3" s="19" t="s">
         <v>24</v>
       </c>
@@ -27827,6 +27827,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:M2"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:T2"/>
+    <mergeCell ref="U1:U3"/>
     <mergeCell ref="AJ1:AN2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -27836,17 +27847,6 @@
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="V1:AI1"/>
-    <mergeCell ref="G1:M2"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="P1:T2"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O22" r:id="rId1"/>
@@ -27959,8 +27959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -27978,10 +27978,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="35.4" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
@@ -28001,8 +28001,8 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="4" t="s">
         <v>564</v>
       </c>
@@ -30347,65 +30347,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="30" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="U1" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="30" t="s">
+      <c r="V1" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="30" t="s">
+      <c r="W1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="30" t="s">
+      <c r="X1" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" s="30" t="s">
+      <c r="Y1" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="30" t="s">
+      <c r="Z1" s="27" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="10" t="s">
         <v>48</v>
       </c>
@@ -30448,13 +30448,13 @@
       <c r="S2" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="25" t="s">
@@ -36854,6 +36854,11 @@
   </sheetData>
   <autoFilter ref="A2:Z102"/>
   <mergeCells count="13">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
@@ -36862,11 +36867,6 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:S1"/>
     <mergeCell ref="T1:T2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Sitios de inspección Ok
</commit_message>
<xml_diff>
--- a/Documentos/Datos.xlsx
+++ b/Documentos/Datos.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7896" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7896" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Rastros(TIF)" sheetId="1" r:id="rId1"/>
     <sheet name="Rastros(Rastro)" sheetId="5" r:id="rId2"/>
     <sheet name="Grupo_mercancia" sheetId="2" r:id="rId3"/>
-    <sheet name="Sitio de inspección" sheetId="3" r:id="rId4"/>
+    <sheet name="Sitio_inspeccion" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Grupo_mercancia!$A$1:$G$101</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Rastros(TIF)'!$A$1:$AN$103</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sitio de inspección'!$A$2:$Z$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sitio_inspeccion!$A$2:$Z$102</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -5608,18 +5608,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5627,6 +5615,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5970,128 +5970,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="1" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="33" t="s">
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="29" t="s">
         <v>1117</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="31" t="s">
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="27" t="s">
         <v>967</v>
       </c>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
     </row>
     <row r="2" spans="1:40" s="1" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="27" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27" t="s">
+      <c r="W2" s="30"/>
+      <c r="X2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27" t="s">
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27" t="s">
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27" t="s">
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="27" t="s">
+      <c r="AE2" s="30"/>
+      <c r="AF2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="27" t="s">
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
     </row>
     <row r="3" spans="1:40" s="1" customFormat="1" ht="24" customHeight="1">
       <c r="A3" s="25" t="s">
@@ -6100,10 +6100,10 @@
       <c r="B3" s="25" t="s">
         <v>1769</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
@@ -6125,8 +6125,8 @@
       <c r="M3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="27"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="30"/>
       <c r="P3" s="18" t="s">
         <v>19</v>
       </c>
@@ -6142,7 +6142,7 @@
       <c r="T3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="33"/>
+      <c r="U3" s="29"/>
       <c r="V3" s="3" t="s">
         <v>24</v>
       </c>
@@ -16830,6 +16830,16 @@
     <filterColumn colId="38" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:M2"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:T2"/>
     <mergeCell ref="AJ1:AN2"/>
     <mergeCell ref="U1:U3"/>
     <mergeCell ref="V1:AI1"/>
@@ -16840,16 +16850,6 @@
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:M2"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="P1:T2"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O22" r:id="rId1"/>
@@ -16996,128 +16996,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="1" customFormat="1" ht="23.4" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="33" t="s">
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="29" t="s">
         <v>1117</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="31" t="s">
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="27" t="s">
         <v>967</v>
       </c>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
     </row>
     <row r="2" spans="1:40" s="1" customFormat="1" ht="23.4" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="27" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27" t="s">
+      <c r="W2" s="30"/>
+      <c r="X2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27" t="s">
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27" t="s">
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27" t="s">
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="27" t="s">
+      <c r="AE2" s="30"/>
+      <c r="AF2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="27" t="s">
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
     </row>
     <row r="3" spans="1:40" s="1" customFormat="1" ht="23.4" customHeight="1">
       <c r="A3" s="25" t="s">
@@ -17126,10 +17126,10 @@
       <c r="B3" s="25" t="s">
         <v>1769</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="20" t="s">
         <v>12</v>
       </c>
@@ -17151,8 +17151,8 @@
       <c r="M3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="27"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="30"/>
       <c r="P3" s="21" t="s">
         <v>19</v>
       </c>
@@ -17168,7 +17168,7 @@
       <c r="T3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="33"/>
+      <c r="U3" s="29"/>
       <c r="V3" s="19" t="s">
         <v>24</v>
       </c>
@@ -27827,17 +27827,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="G1:M2"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="P1:T2"/>
-    <mergeCell ref="U1:U3"/>
     <mergeCell ref="AJ1:AN2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -27847,6 +27836,17 @@
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="V1:AI1"/>
+    <mergeCell ref="G1:M2"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:T2"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O22" r:id="rId1"/>
@@ -27959,7 +27959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -27978,10 +27978,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="35.4" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
@@ -28001,8 +28001,8 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="4" t="s">
         <v>564</v>
       </c>
@@ -30318,7 +30318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -30347,65 +30347,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="27" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Y1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="Z1" s="30" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="14" customFormat="1" ht="18" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="10" t="s">
         <v>48</v>
       </c>
@@ -30448,13 +30448,13 @@
       <c r="S2" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="25" t="s">
@@ -36854,11 +36854,6 @@
   </sheetData>
   <autoFilter ref="A2:Z102"/>
   <mergeCells count="13">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
@@ -36867,6 +36862,11 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:S1"/>
     <mergeCell ref="T1:T2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>